<commit_message>
Excel version of metadata templates
</commit_message>
<xml_diff>
--- a/edi_2021/metadata_templates/metadata_attributes.xlsx
+++ b/edi_2021/metadata_templates/metadata_attributes.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpien\OneDrive - California Department of Water Resources\Work\Database\DataPublication\publish_fish\edi_2021\metadata_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/catarina_pien_water_ca_gov/Documents/Work/Database/DataPublication/publish_fish/edi_2021/metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DDA53C-2E8D-4C0A-BB93-457EFA15E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{19DDA53C-2E8D-4C0A-BB93-457EFA15E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13BA568A-254D-4317-8B6C-00480FAF0A5F}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1260" windowWidth="21600" windowHeight="11385" tabRatio="793" firstSheet="5" activeTab="9" xr2:uid="{7E51937F-B94B-4653-9E6F-42F95F9832B9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="793" firstSheet="3" activeTab="5" xr2:uid="{7E51937F-B94B-4653-9E6F-42F95F9832B9}"/>
   </bookViews>
   <sheets>
     <sheet name="attributes_effort" sheetId="1" r:id="rId1"/>
     <sheet name="attributes_event" sheetId="2" r:id="rId2"/>
     <sheet name="attributes_fish_unique" sheetId="3" r:id="rId3"/>
     <sheet name="attributes_genetics_salmon" sheetId="4" r:id="rId4"/>
-    <sheet name="attributes_genetics_smelt" sheetId="5" r:id="rId5"/>
-    <sheet name="attributes_integrated_wq_totalc" sheetId="6" r:id="rId6"/>
-    <sheet name="attributes_monthly_trap_effort" sheetId="10" r:id="rId7"/>
-    <sheet name="attributes_station" sheetId="7" r:id="rId8"/>
-    <sheet name="attributes_taxonomy" sheetId="8" r:id="rId9"/>
+    <sheet name="attributes_integrated_wq_totalc" sheetId="6" r:id="rId5"/>
+    <sheet name="attributes_intwq" sheetId="12" r:id="rId6"/>
+    <sheet name="attributes_genetics_smelt" sheetId="5" r:id="rId7"/>
+    <sheet name="attributes_monthly_trap_effort" sheetId="10" r:id="rId8"/>
+    <sheet name="attributes_station" sheetId="7" r:id="rId9"/>
     <sheet name="attributes_total_catch" sheetId="9" r:id="rId10"/>
+    <sheet name="attributes_taxonomy" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="190">
   <si>
     <t>attributeName</t>
   </si>
@@ -303,9 +304,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>cubicmeter</t>
-  </si>
-  <si>
     <t>hour</t>
   </si>
   <si>
@@ -610,6 +608,12 @@
   </si>
   <si>
     <t>No comments recorded</t>
+  </si>
+  <si>
+    <t>cubicMeter</t>
+  </si>
+  <si>
+    <t>IEP Fish Code</t>
   </si>
 </sst>
 </file>
@@ -964,20 +968,20 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,23 +1004,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1027,13 +1031,16 @@
       <c r="F3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1045,15 +1052,15 @@
         <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1065,35 +1072,35 @@
         <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="F6" t="s">
         <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -1102,27 +1109,27 @@
         <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
         <v>128</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1134,21 +1141,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D918347C-D870-411E-BE76-C372E2C4C941}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1171,40 +1178,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1215,7 +1222,213 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8F4E1E-15C5-4057-B218-3679BBC105A9}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1227,22 +1440,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B7538F-154B-4513-A210-38D51A4AF510}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="A1:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1265,182 +1478,182 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
         <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
         <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
         <v>85</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>98</v>
-      </c>
       <c r="F10" t="s">
         <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
         <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -1452,15 +1665,15 @@
         <v>85</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1469,15 +1682,15 @@
         <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1486,15 +1699,15 @@
         <v>85</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -1503,15 +1716,15 @@
         <v>85</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1520,15 +1733,15 @@
         <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1537,15 +1750,15 @@
         <v>85</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1554,15 +1767,15 @@
         <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1571,15 +1784,15 @@
         <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1588,15 +1801,15 @@
         <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1605,15 +1818,15 @@
         <v>85</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1622,40 +1835,43 @@
         <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -1671,21 +1887,21 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F15"/>
+      <selection activeCell="G15" sqref="A1:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1708,23 +1924,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -1733,66 +1949,66 @@
         <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" t="s">
         <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1803,16 +2019,16 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1826,15 +2042,15 @@
         <v>85</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1843,15 +2059,15 @@
         <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -1860,15 +2076,15 @@
         <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1877,15 +2093,15 @@
         <v>85</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1894,15 +2110,15 @@
         <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1911,21 +2127,24 @@
         <v>85</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
       <c r="G15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1938,21 +2157,21 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1975,34 +2194,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -2011,35 +2230,35 @@
         <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
         <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -2048,49 +2267,52 @@
         <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" t="s">
         <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
       <c r="G8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2102,6 +2324,1095 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B51B647-CAD3-4E61-B397-F0AD4BA7FD9D}">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A172CD93-F435-4FC7-BD7F-D28212A95F69}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E88073-8B38-4800-AC59-10539A2946B6}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -2109,18 +3420,18 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2143,94 +3454,94 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
         <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
         <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
         <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -2239,15 +3550,15 @@
         <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -2259,21 +3570,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B51B647-CAD3-4E61-B397-F0AD4BA7FD9D}">
-  <dimension ref="A1:G32"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF98D43F-E88A-462F-B559-325C0DF510A4}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F32"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2296,498 +3610,71 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
         <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
         <v>187</v>
-      </c>
-      <c r="B18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>119</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" t="s">
-        <v>182</v>
-      </c>
-      <c r="C26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
-        <v>186</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s">
-        <v>127</v>
-      </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2795,116 +3682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF98D43F-E88A-462F-B559-325C0DF510A4}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C5F487-6D18-41FD-AAC9-E024241FDE76}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -2912,18 +3690,18 @@
       <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2946,315 +3724,109 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>70</v>
       </c>
       <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>160</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8F4E1E-15C5-4057-B218-3679BBC105A9}">
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" t="s">
-        <v>175</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>